<commit_message>
Replacing "meat bag" with "humanoid" for professional reasons
</commit_message>
<xml_diff>
--- a/docs/05_botiumscript/media/excel/helloworld_namedconvos.xlsx
+++ b/docs/05_botiumscript/media/excel/helloworld_namedconvos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Convos - HelloWorld" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t xml:space="preserve">Test Case</t>
   </si>
@@ -39,13 +39,44 @@
     <t xml:space="preserve">hello bot!</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello, meat bag! How can I help you ?</t>
+    <t xml:space="preserve">Hello, humanoid! How can I help you ?</t>
   </si>
   <si>
     <t xml:space="preserve">TC02_HELLO_DUDE</t>
   </si>
   <si>
     <t xml:space="preserve">hey dude</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Hello, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">humanoid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">! How can I help you ?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">TC03_HELLO</t>
@@ -98,7 +129,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -128,6 +159,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -222,11 +259,11 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.44"/>
@@ -267,7 +304,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -288,11 +325,11 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.44"/>
@@ -312,28 +349,28 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -358,7 +395,7 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.3359375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.34375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.55"/>
@@ -366,15 +403,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>
@@ -382,7 +419,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -392,40 +429,40 @@
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>